<commit_message>
using max date for ihme instead of previous 08-04 projection date
</commit_message>
<xml_diff>
--- a/data/raw/2020-05-04/sheet_all_tabs.xlsx
+++ b/data/raw/2020-05-04/sheet_all_tabs.xlsx
@@ -1312,7 +1312,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -1352,7 +1352,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -1392,7 +1392,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -1472,7 +1472,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -1512,7 +1512,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1592,7 +1592,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1632,7 +1632,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1672,7 +1672,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1712,7 +1712,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1752,7 +1752,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1832,7 +1832,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1872,7 +1872,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1912,7 +1912,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1952,7 +1952,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1992,7 +1992,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -2072,7 +2072,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">

</xml_diff>